<commit_message>
integrate web design from figma
</commit_message>
<xml_diff>
--- a/public-totem/card file/prophecy of the totem card info.xlsx
+++ b/public-totem/card file/prophecy of the totem card info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git projects\simple-game-portfolio\prophecy of the totem\card file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git projects\simple-game-portfolio\public-totem\card file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11C8631-4FBF-45FB-AEA3-540B70818540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642BFF8E-21BB-47E8-AA15-F2DC61C28931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="599" activeTab="2" xr2:uid="{F566331A-B89A-4A41-9B13-9C3484F3F3A2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
   <si>
     <t>予言カード名</t>
   </si>
@@ -343,30 +343,18 @@
     <t>破壊のクロー</t>
   </si>
   <si>
-    <t>任意のプレイヤー1名がトーテムに置いたパーツカードをひとつ破棄する。</t>
-  </si>
-  <si>
     <t>衰退のオーブ</t>
   </si>
   <si>
-    <t>任意のプレイヤー1名に手札一枚捨てさせる。</t>
-  </si>
-  <si>
     <t>干渉の鎖</t>
   </si>
   <si>
     <t>連動アーム</t>
   </si>
   <si>
-    <t>自分のトーテムにある、逆側の腕についているパーツカードの効果を追加で1回発動する。</t>
-  </si>
-  <si>
     <t>連動レッグ</t>
   </si>
   <si>
-    <t>自分のトーテムにある、逆側の足についているパーツカードの効果を追加で1回発動する。</t>
-  </si>
-  <si>
     <t>追跡の眼</t>
   </si>
   <si>
@@ -382,15 +370,9 @@
     <t>探求の書</t>
   </si>
   <si>
-    <t>山札からパーツカードを3枚引き、その中から好きな1枚を選んで手札に加える。</t>
-  </si>
-  <si>
     <t>強奪のグローブ</t>
   </si>
   <si>
-    <t>任意のプレイヤー1名からカードをひとつ引いて手札に加える。</t>
-  </si>
-  <si>
     <t>発動のコア</t>
   </si>
   <si>
@@ -415,9 +397,6 @@
     <t>手札のパーツカードを2枚捨てて、任意のプレイヤー1名のプレイヤートーテムにあるパーツカードを自分の手札に加える。</t>
   </si>
   <si>
-    <t>この効果は配置時のみ使える。他のプレイヤー1人の予言カードを確認できる。</t>
-  </si>
-  <si>
     <t>覚醒している枠にある限り、効果は永続。セントラルトーテムに自分のジェムを追加する手札コストを1枚減らす。</t>
   </si>
   <si>
@@ -427,13 +406,40 @@
     <t>自分の手札枚数を8にする。</t>
   </si>
   <si>
-    <t>　</t>
-  </si>
-  <si>
     <t>知識の破片</t>
   </si>
   <si>
     <t>知識の産物</t>
+  </si>
+  <si>
+    <t>この効果は配置時のみ使える。任意のプレイヤー1名がトーテムに置いたパーツカードをひとつ破棄する。</t>
+  </si>
+  <si>
+    <t>この効果は配置時のみ使える。プレイヤー二人まで選び、その二人の手札から2枚見ずに捨てさせる。</t>
+  </si>
+  <si>
+    <t>プレイヤーを一人選び、それぞれ手札1枚選ぶ。それを交換する。</t>
+  </si>
+  <si>
+    <t>自分のトーテムにある、逆側の羽についているパーツカードの効果を追加で1回発動する。</t>
+  </si>
+  <si>
+    <t>他のプレイヤー1人の手札を確認できる。</t>
+  </si>
+  <si>
+    <t>このカードが配置されている枠と同じ枠に配置されている相手のパーツカードをすべて破壊する。</t>
+  </si>
+  <si>
+    <t>自分のジェムをすべて破棄し、すべてのプレイヤーの手札を捨て、自分のみカードを4枚引く</t>
+  </si>
+  <si>
+    <t>自分の配置されているパーツカード1枚と任意のプレイヤーのパーツカードを1枚指定し、それらを破壊する。</t>
+  </si>
+  <si>
+    <t>任意のプレイヤー1名からカードをひとつ見ずに手札に加える。</t>
+  </si>
+  <si>
+    <t>山札からパーツカードを3枚引き、その中から好きな1枚を選んで手札に加える。残りはデッキに戻してシャッフルする。</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,8 +488,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFABAB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFEC6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -521,11 +557,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -535,14 +582,33 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFABAB"/>
+      <color rgb="FFFAFEC6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1121,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BC1D7B-E04D-47F8-AB3F-9CE10226F913}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1316,7 @@
         <v>71</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>53</v>
@@ -1434,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30586910-A6A8-4F0E-8A41-B23759FDAA7C}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1513,7 @@
     <col min="3" max="3" width="114.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>87</v>
       </c>
@@ -1462,246 +1528,312 @@
       </c>
       <c r="E1">
         <f>SUM(E2,E7,E14)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="G1">
+        <f>SUM(G2:G6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="5">
-        <v>8</v>
+      <c r="D2">
+        <v>10</v>
       </c>
       <c r="E2">
         <f>SUM(D2:D6)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="F2" s="16">
+        <f>SUM(D2,D3,D14,D15,D18)</f>
+        <v>30</v>
+      </c>
+      <c r="G2" s="19">
+        <f t="shared" ref="G2:G6" si="0">F2/$E$1</f>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="F3" s="17">
+        <f>SUM(D5,D6,D9,D10,D17)</f>
+        <v>28</v>
+      </c>
+      <c r="G3" s="19">
+        <f t="shared" si="0"/>
+        <v>0.25454545454545452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="15">
+        <f>SUM(D4,D11,D12,D13,D16)</f>
+        <v>22</v>
+      </c>
+      <c r="G4" s="19">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="F5" s="11">
+        <f>SUM(D8,D19,D21)</f>
+        <v>12</v>
+      </c>
+      <c r="G5" s="19">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="F6" s="18">
+        <f>SUM(D7,D20,D22)</f>
+        <v>18</v>
+      </c>
+      <c r="G6" s="19">
+        <f t="shared" si="0"/>
+        <v>0.16363636363636364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="5">
-        <v>5</v>
+      <c r="C7" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
       </c>
       <c r="E7">
         <f>SUM(D7:D13)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D9" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="5">
-        <v>2</v>
+        <v>123</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
       </c>
       <c r="E14">
-        <f>SUM(D14:D19)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>SUM(D14:D22)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="5">
-        <v>2</v>
+        <v>110</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="D17">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="5">
-        <v>2</v>
+        <v>112</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="5">
+        <v>114</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="6" t="s">
-        <v>129</v>
+      <c r="C22" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>